<commit_message>
timings for the sync feature
</commit_message>
<xml_diff>
--- a/lid/timing.xlsx
+++ b/lid/timing.xlsx
@@ -12,25 +12,19 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Open-sec</t>
+    <t>Open</t>
   </si>
   <si>
-    <t>frames</t>
-  </si>
-  <si>
-    <t>close-sec</t>
-  </si>
-  <si>
-    <t>ms</t>
+    <t>Close</t>
   </si>
 </sst>
 </file>
@@ -371,165 +365,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G7"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
-        <v>0</v>
+        <v>467</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>B2/29</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <f>INT((E2+(F2/29))*1000)</f>
-        <v>4862</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>A2+600</f>
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
-        <v>5</v>
+        <v>2102</v>
       </c>
       <c r="B3">
-        <v>28</v>
-      </c>
-      <c r="C3">
-        <f>INT((A3+(B3/29))*1000)</f>
-        <v>5965</v>
-      </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <f>INT((E3+(F3/29))*1000)</f>
-        <v>9517</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>A3+600</f>
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
-        <v>9</v>
+        <v>3470</v>
       </c>
       <c r="B4">
-        <v>28</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C7" si="0">INT((A4+(B4/29))*1000)</f>
-        <v>9965</v>
-      </c>
-      <c r="E4">
-        <v>16</v>
-      </c>
-      <c r="F4">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G7" si="1">INT((E4+(F4/29))*1000)</f>
-        <v>16862</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>A4+600</f>
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
-        <v>17</v>
+        <v>5038</v>
       </c>
       <c r="B5">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>17793</v>
-      </c>
-      <c r="E5">
-        <v>21</v>
-      </c>
-      <c r="F5">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
-        <v>21586</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>A5+600</f>
+        <v>5638</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
-        <v>22</v>
+        <v>6673</v>
       </c>
       <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>22275</v>
-      </c>
-      <c r="E6">
-        <v>23</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>28</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>23965</v>
-      </c>
-      <c r="E7">
-        <v>24</v>
-      </c>
-      <c r="F7">
-        <v>29</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>25000</v>
+        <f>A6+600</f>
+        <v>7273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>